<commit_message>
Added Model login logout timesheet
</commit_message>
<xml_diff>
--- a/Input/KPO-BPO December HC_2Jan'23.xlsx
+++ b/Input/KPO-BPO December HC_2Jan'23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BCTPK1\Documents\BCTTimesheet\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450FEC26-DCD8-42C1-B294-6C0682DB944B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ACF3B3-66B4-4AE5-B93D-EFC9250F25AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E587A84D-F539-48CF-B31A-8D1EE02B8D4B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Exit" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Client Details'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Client Details'!$B$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">HC!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1641,25 +1641,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>329</v>
@@ -1667,129 +1667,129 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>21220</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B3" s="1">
-        <v>21254</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>284</v>
+        <v>284</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="1">
+        <v>21254</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>21339</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" s="16">
         <v>28743</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="B6" s="16">
+      <c r="C6" s="16">
         <v>52003</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>52005</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="B8" s="16">
+      <c r="C8" s="16">
         <v>52007</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>52013</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>52015</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="1">
         <v>90007</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C12" s="1">
         <v>99053</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>282</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C12" xr:uid="{814C04A6-47AD-48AF-BBF9-BBADFC70B9FF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
-      <sortCondition ref="B1:B12"/>
+  <autoFilter ref="B1:C12" xr:uid="{814C04A6-47AD-48AF-BBF9-BBADFC70B9FF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C12">
+      <sortCondition ref="C1:C12"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>